<commit_message>
Correction orthographe Ajout menu dans les fichiers excel pour trier chaque catégorie Ajout d'une fonction permettant d'effectuer un tri par ordre alphabétique par défaut correction bug noah loss extractor dans le cas ou on etait sur la page audiométrie vocale. Augmentation robustesse de la fonction dans ce cas pour éviter plantage. Double changement dans le main pour forcer le passage à la bonne page audiométrie tonale. Changement couleur plus foncé pour la synthèse. Correction bug qui n'affichait pas dans la synthèse lorsque appareil si besoin ressenti
</commit_message>
<xml_diff>
--- a/mode_test/fichier_test/Liste Referents.xlsx
+++ b/mode_test/fichier_test/Liste Referents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audio69\Documents\DocOdipro\DocMaster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audio69\PycharmProjects\turtle\mode_test\fichier_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C575AA79-E35E-4EC2-89BD-7770320C4468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00823D0D-CF86-4B4E-B2E3-1DBE6392415B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>LISTE DES REFERENTS</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Mail</t>
   </si>
   <si>
-    <t>Propriété exclusive de la SASU NVCM - ODIPRO</t>
-  </si>
-  <si>
     <t>Empreinte</t>
   </si>
 </sst>
@@ -50,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -58,11 +55,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -448,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -474,103 +466,100 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -906,23 +895,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="38"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="19"/>
-      <c r="I2" s="40"/>
+      <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:9" s="8" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -945,8 +934,8 @@
       <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="41" t="s">
-        <v>7</v>
+      <c r="I3" s="35" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1274,30 +1263,30 @@
       <c r="H28" s="30"/>
       <c r="I28" s="30"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
+    <row r="29" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>26</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D45"/>
       <c r="G45"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A29:H29"/>
     <mergeCell ref="D2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D28" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D29" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Epoux(se),Fille/Fils,Tuteur/Curateur,Sœur/Frère,Nièce/Neuveu,Ami(e)"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Correction bug dans le noah loss extractor qui amenait dans certains moment à mal gérer les personnes avec une audition normale. Correction bug pour les perte de 20 dB Adjonction d'un module qui permet de faire la distinction entre l'audiogramme calisto en mode simple ou double. ++ Ajout d'une fonctionalité récupération des données qui va directement integrer les fichier temporaire à la session actuelle Ajout de la commande F3 qui permet de fermer la session sans sauvegarde ni fusion pdf ni zippage ce qui permet de reprendre la session en cas de bug ou de depistage sur plusieurs jours ou si on souhaite finir de remplir les tableaux à un autre moment. Sur l'affichage fenetre maison retraite ajout d'option bloquante permettant d'éviter de rentrer plusieurs maison de retraite A la demande d'Elisabeth refonte de la partie commentaire dans le fenetre  anamnese. Remplacement de entry par text + adjonction d'un texte wrapper dans la fenetre et pour la redaction du commentaire
</commit_message>
<xml_diff>
--- a/mode_test/fichier_test/Liste Referents.xlsx
+++ b/mode_test/fichier_test/Liste Referents.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audio69\PycharmProjects\turtle\mode_test\fichier_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00823D0D-CF86-4B4E-B2E3-1DBE6392415B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC5A5FE-67BB-4749-8856-730BDB6E5A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -440,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,6 +557,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -874,42 +888,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I203"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="32" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="33" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="33" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" style="33" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="33" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="33" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="33" customWidth="1"/>
     <col min="9" max="12" width="11.5703125" style="33" customWidth="1"/>
     <col min="13" max="16384" width="11.5703125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="G2" s="19"/>
       <c r="I2" s="34"/>
     </row>
@@ -1276,9 +1290,2441 @@
       <c r="H29" s="30"/>
       <c r="I29" s="30"/>
     </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D45"/>
-      <c r="G45"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="36">
+        <f>A29+1</f>
+        <v>27</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="36">
+        <f t="shared" ref="A31:A94" si="0">A30+1</f>
+        <v>28</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="36">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="36">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="36">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="36">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="36">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="36">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="36">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="36">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="36">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="36">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="36">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="36">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="36">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="36">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="36">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="36">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="36">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="36">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="36">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="36">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="36">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="36">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="36">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="36">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="36">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="36">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="36">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="36">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="36">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="36">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="36">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="36">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="36">
+        <f>A65+1</f>
+        <v>63</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="36">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="36">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="36">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="36">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="36">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="36">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="36">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="36">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="36">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="36">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="36">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="36">
+        <f>A77+1</f>
+        <v>75</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="36">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="36">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="36">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="36">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="36">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="36">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="36">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="36">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="36">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="36">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="36">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="36">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="36">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="36">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="36">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="36">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="36">
+        <f t="shared" ref="A95:A101" si="1">A94+1</f>
+        <v>92</v>
+      </c>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="36">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="36">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="36">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="36">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="36">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="36">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="36">
+        <f>A101+1</f>
+        <v>99</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+      <c r="I102" s="10"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="36">
+        <f>A102+1</f>
+        <v>100</v>
+      </c>
+      <c r="B103" s="10"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="36">
+        <f t="shared" ref="A104:A166" si="2">A103+1</f>
+        <v>101</v>
+      </c>
+      <c r="B104" s="10"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="36">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="36">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" s="36">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="36">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="36">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="36">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="B110" s="10"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="36">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="36">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="36">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
+      <c r="I113" s="10"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="36">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="B114" s="10"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="10"/>
+      <c r="G114" s="10"/>
+      <c r="H114" s="10"/>
+      <c r="I114" s="10"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="36">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="36">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="B116" s="10"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="10"/>
+      <c r="F116" s="10"/>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
+      <c r="I116" s="10"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="36">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="B117" s="10"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="36">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="B118" s="10"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="10"/>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+      <c r="I118" s="10"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="36">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="B119" s="10"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="10"/>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+      <c r="I119" s="10"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="36">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="B120" s="10"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+      <c r="G120" s="10"/>
+      <c r="H120" s="10"/>
+      <c r="I120" s="10"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="36">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="36">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" s="36">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="36">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="B124" s="10"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="36">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="36">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+      <c r="B126" s="10"/>
+      <c r="C126" s="10"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="10"/>
+      <c r="F126" s="10"/>
+      <c r="G126" s="10"/>
+      <c r="H126" s="10"/>
+      <c r="I126" s="10"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="36">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="36">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="B128" s="10"/>
+      <c r="C128" s="10"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="10"/>
+      <c r="G128" s="10"/>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="36">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="36">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="B130" s="10"/>
+      <c r="C130" s="10"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" s="36">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" s="36">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" s="36">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="B133" s="10"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="10"/>
+      <c r="G133" s="10"/>
+      <c r="H133" s="10"/>
+      <c r="I133" s="10"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" s="36">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="B134" s="10"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+      <c r="G134" s="10"/>
+      <c r="H134" s="10"/>
+      <c r="I134" s="10"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" s="36">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="B135" s="10"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="10"/>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" s="36">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="B136" s="10"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="10"/>
+      <c r="G136" s="10"/>
+      <c r="H136" s="10"/>
+      <c r="I136" s="10"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="36">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="B137" s="10"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" s="36">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="B138" s="10"/>
+      <c r="C138" s="10"/>
+      <c r="D138" s="10"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10"/>
+      <c r="G138" s="10"/>
+      <c r="H138" s="10"/>
+      <c r="I138" s="10"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" s="36">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="B139" s="10"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" s="36">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="H140" s="10"/>
+      <c r="I140" s="10"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" s="36">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" s="36">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="B142" s="10"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10"/>
+      <c r="H142" s="10"/>
+      <c r="I142" s="10"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" s="36">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A144" s="36">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="10"/>
+      <c r="G144" s="10"/>
+      <c r="H144" s="10"/>
+      <c r="I144" s="10"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" s="36">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="10"/>
+      <c r="G145" s="10"/>
+      <c r="H145" s="10"/>
+      <c r="I145" s="10"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A146" s="36">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="B146" s="10"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="10"/>
+      <c r="G146" s="10"/>
+      <c r="H146" s="10"/>
+      <c r="I146" s="10"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A147" s="36">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A148" s="36">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
+      <c r="F148" s="10"/>
+      <c r="G148" s="10"/>
+      <c r="H148" s="10"/>
+      <c r="I148" s="10"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" s="36">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
+      <c r="F149" s="10"/>
+      <c r="G149" s="10"/>
+      <c r="H149" s="10"/>
+      <c r="I149" s="10"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="36">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="B150" s="10"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
+      <c r="F150" s="10"/>
+      <c r="G150" s="10"/>
+      <c r="H150" s="10"/>
+      <c r="I150" s="10"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A151" s="36">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
+      <c r="F151" s="10"/>
+      <c r="G151" s="10"/>
+      <c r="H151" s="10"/>
+      <c r="I151" s="10"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" s="36">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="B152" s="10"/>
+      <c r="C152" s="10"/>
+      <c r="D152" s="10"/>
+      <c r="E152" s="10"/>
+      <c r="F152" s="10"/>
+      <c r="G152" s="10"/>
+      <c r="H152" s="10"/>
+      <c r="I152" s="10"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" s="36">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="B153" s="10"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
+      <c r="F153" s="10"/>
+      <c r="G153" s="10"/>
+      <c r="H153" s="10"/>
+      <c r="I153" s="10"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="36">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="B154" s="10"/>
+      <c r="C154" s="10"/>
+      <c r="D154" s="10"/>
+      <c r="E154" s="10"/>
+      <c r="F154" s="10"/>
+      <c r="G154" s="10"/>
+      <c r="H154" s="10"/>
+      <c r="I154" s="10"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" s="36">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="B155" s="10"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+      <c r="F155" s="10"/>
+      <c r="G155" s="10"/>
+      <c r="H155" s="10"/>
+      <c r="I155" s="10"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A156" s="36">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="B156" s="10"/>
+      <c r="C156" s="10"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="10"/>
+      <c r="F156" s="10"/>
+      <c r="G156" s="10"/>
+      <c r="H156" s="10"/>
+      <c r="I156" s="10"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A157" s="36">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="B157" s="10"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10"/>
+      <c r="G157" s="10"/>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A158" s="36">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="B158" s="10"/>
+      <c r="C158" s="10"/>
+      <c r="D158" s="10"/>
+      <c r="E158" s="10"/>
+      <c r="F158" s="10"/>
+      <c r="G158" s="10"/>
+      <c r="H158" s="10"/>
+      <c r="I158" s="10"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" s="36">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="B159" s="10"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+      <c r="F159" s="10"/>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A160" s="36">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="B160" s="10"/>
+      <c r="C160" s="10"/>
+      <c r="D160" s="10"/>
+      <c r="E160" s="10"/>
+      <c r="F160" s="10"/>
+      <c r="G160" s="10"/>
+      <c r="H160" s="10"/>
+      <c r="I160" s="10"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A161" s="36">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="B161" s="10"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
+      <c r="F161" s="10"/>
+      <c r="G161" s="10"/>
+      <c r="H161" s="10"/>
+      <c r="I161" s="10"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="36">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="B162" s="10"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
+      <c r="F162" s="10"/>
+      <c r="G162" s="10"/>
+      <c r="H162" s="10"/>
+      <c r="I162" s="10"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A163" s="36">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+      <c r="F163" s="10"/>
+      <c r="G163" s="10"/>
+      <c r="H163" s="10"/>
+      <c r="I163" s="10"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A164" s="36">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="B164" s="10"/>
+      <c r="C164" s="10"/>
+      <c r="D164" s="10"/>
+      <c r="E164" s="10"/>
+      <c r="F164" s="10"/>
+      <c r="G164" s="10"/>
+      <c r="H164" s="10"/>
+      <c r="I164" s="10"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" s="36">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="B165" s="10"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
+      <c r="F165" s="10"/>
+      <c r="G165" s="10"/>
+      <c r="H165" s="10"/>
+      <c r="I165" s="10"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" s="36">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+      <c r="B166" s="10"/>
+      <c r="C166" s="10"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="10"/>
+      <c r="F166" s="10"/>
+      <c r="G166" s="10"/>
+      <c r="H166" s="10"/>
+      <c r="I166" s="10"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" s="36">
+        <f t="shared" ref="A167:A203" si="3">A166+1</f>
+        <v>164</v>
+      </c>
+      <c r="B167" s="10"/>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
+      <c r="F167" s="10"/>
+      <c r="G167" s="10"/>
+      <c r="H167" s="10"/>
+      <c r="I167" s="10"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A168" s="36">
+        <f t="shared" si="3"/>
+        <v>165</v>
+      </c>
+      <c r="B168" s="10"/>
+      <c r="C168" s="10"/>
+      <c r="D168" s="10"/>
+      <c r="E168" s="10"/>
+      <c r="F168" s="10"/>
+      <c r="G168" s="10"/>
+      <c r="H168" s="10"/>
+      <c r="I168" s="10"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A169" s="36">
+        <f t="shared" si="3"/>
+        <v>166</v>
+      </c>
+      <c r="B169" s="10"/>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
+      <c r="F169" s="10"/>
+      <c r="G169" s="10"/>
+      <c r="H169" s="10"/>
+      <c r="I169" s="10"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A170" s="36">
+        <f t="shared" si="3"/>
+        <v>167</v>
+      </c>
+      <c r="B170" s="10"/>
+      <c r="C170" s="10"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="10"/>
+      <c r="F170" s="10"/>
+      <c r="G170" s="10"/>
+      <c r="H170" s="10"/>
+      <c r="I170" s="10"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A171" s="36">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="B171" s="10"/>
+      <c r="C171" s="10"/>
+      <c r="D171" s="10"/>
+      <c r="E171" s="10"/>
+      <c r="F171" s="10"/>
+      <c r="G171" s="10"/>
+      <c r="H171" s="10"/>
+      <c r="I171" s="10"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A172" s="36">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="B172" s="10"/>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
+      <c r="F172" s="10"/>
+      <c r="G172" s="10"/>
+      <c r="H172" s="10"/>
+      <c r="I172" s="10"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A173" s="36">
+        <f t="shared" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="B173" s="10"/>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="10"/>
+      <c r="F173" s="10"/>
+      <c r="G173" s="10"/>
+      <c r="H173" s="10"/>
+      <c r="I173" s="10"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A174" s="36">
+        <f t="shared" si="3"/>
+        <v>171</v>
+      </c>
+      <c r="B174" s="10"/>
+      <c r="C174" s="10"/>
+      <c r="D174" s="10"/>
+      <c r="E174" s="10"/>
+      <c r="F174" s="10"/>
+      <c r="G174" s="10"/>
+      <c r="H174" s="10"/>
+      <c r="I174" s="10"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A175" s="36">
+        <f t="shared" si="3"/>
+        <v>172</v>
+      </c>
+      <c r="B175" s="10"/>
+      <c r="C175" s="10"/>
+      <c r="D175" s="10"/>
+      <c r="E175" s="10"/>
+      <c r="F175" s="10"/>
+      <c r="G175" s="10"/>
+      <c r="H175" s="10"/>
+      <c r="I175" s="10"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A176" s="36">
+        <f t="shared" si="3"/>
+        <v>173</v>
+      </c>
+      <c r="B176" s="10"/>
+      <c r="C176" s="10"/>
+      <c r="D176" s="10"/>
+      <c r="E176" s="10"/>
+      <c r="F176" s="10"/>
+      <c r="G176" s="10"/>
+      <c r="H176" s="10"/>
+      <c r="I176" s="10"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A177" s="36">
+        <f t="shared" si="3"/>
+        <v>174</v>
+      </c>
+      <c r="B177" s="10"/>
+      <c r="C177" s="10"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="10"/>
+      <c r="F177" s="10"/>
+      <c r="G177" s="10"/>
+      <c r="H177" s="10"/>
+      <c r="I177" s="10"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A178" s="36">
+        <f t="shared" si="3"/>
+        <v>175</v>
+      </c>
+      <c r="B178" s="10"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
+      <c r="F178" s="10"/>
+      <c r="G178" s="10"/>
+      <c r="H178" s="10"/>
+      <c r="I178" s="10"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A179" s="36">
+        <f t="shared" si="3"/>
+        <v>176</v>
+      </c>
+      <c r="B179" s="10"/>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
+      <c r="F179" s="10"/>
+      <c r="G179" s="10"/>
+      <c r="H179" s="10"/>
+      <c r="I179" s="10"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A180" s="36">
+        <f t="shared" si="3"/>
+        <v>177</v>
+      </c>
+      <c r="B180" s="10"/>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
+      <c r="F180" s="10"/>
+      <c r="G180" s="10"/>
+      <c r="H180" s="10"/>
+      <c r="I180" s="10"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A181" s="36">
+        <f t="shared" si="3"/>
+        <v>178</v>
+      </c>
+      <c r="B181" s="10"/>
+      <c r="C181" s="10"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
+      <c r="F181" s="10"/>
+      <c r="G181" s="10"/>
+      <c r="H181" s="10"/>
+      <c r="I181" s="10"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A182" s="36">
+        <f t="shared" si="3"/>
+        <v>179</v>
+      </c>
+      <c r="B182" s="10"/>
+      <c r="C182" s="10"/>
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
+      <c r="F182" s="10"/>
+      <c r="G182" s="10"/>
+      <c r="H182" s="10"/>
+      <c r="I182" s="10"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A183" s="36">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="B183" s="10"/>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
+      <c r="F183" s="10"/>
+      <c r="G183" s="10"/>
+      <c r="H183" s="10"/>
+      <c r="I183" s="10"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A184" s="36">
+        <f t="shared" si="3"/>
+        <v>181</v>
+      </c>
+      <c r="B184" s="10"/>
+      <c r="C184" s="10"/>
+      <c r="D184" s="10"/>
+      <c r="E184" s="10"/>
+      <c r="F184" s="10"/>
+      <c r="G184" s="10"/>
+      <c r="H184" s="10"/>
+      <c r="I184" s="10"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A185" s="36">
+        <f t="shared" si="3"/>
+        <v>182</v>
+      </c>
+      <c r="B185" s="10"/>
+      <c r="C185" s="10"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
+      <c r="F185" s="10"/>
+      <c r="G185" s="10"/>
+      <c r="H185" s="10"/>
+      <c r="I185" s="10"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A186" s="36">
+        <f t="shared" si="3"/>
+        <v>183</v>
+      </c>
+      <c r="B186" s="10"/>
+      <c r="C186" s="10"/>
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
+      <c r="F186" s="10"/>
+      <c r="G186" s="10"/>
+      <c r="H186" s="10"/>
+      <c r="I186" s="10"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A187" s="36">
+        <f t="shared" si="3"/>
+        <v>184</v>
+      </c>
+      <c r="B187" s="10"/>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
+      <c r="F187" s="10"/>
+      <c r="G187" s="10"/>
+      <c r="H187" s="10"/>
+      <c r="I187" s="10"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A188" s="36">
+        <f t="shared" si="3"/>
+        <v>185</v>
+      </c>
+      <c r="B188" s="10"/>
+      <c r="C188" s="10"/>
+      <c r="D188" s="10"/>
+      <c r="E188" s="10"/>
+      <c r="F188" s="10"/>
+      <c r="G188" s="10"/>
+      <c r="H188" s="10"/>
+      <c r="I188" s="10"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="36">
+        <f t="shared" si="3"/>
+        <v>186</v>
+      </c>
+      <c r="B189" s="10"/>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
+      <c r="F189" s="10"/>
+      <c r="G189" s="10"/>
+      <c r="H189" s="10"/>
+      <c r="I189" s="10"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A190" s="36">
+        <f t="shared" si="3"/>
+        <v>187</v>
+      </c>
+      <c r="B190" s="10"/>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="10"/>
+      <c r="F190" s="10"/>
+      <c r="G190" s="10"/>
+      <c r="H190" s="10"/>
+      <c r="I190" s="10"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A191" s="36">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="B191" s="10"/>
+      <c r="C191" s="10"/>
+      <c r="D191" s="10"/>
+      <c r="E191" s="10"/>
+      <c r="F191" s="10"/>
+      <c r="G191" s="10"/>
+      <c r="H191" s="10"/>
+      <c r="I191" s="10"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A192" s="36">
+        <f t="shared" si="3"/>
+        <v>189</v>
+      </c>
+      <c r="B192" s="10"/>
+      <c r="C192" s="10"/>
+      <c r="D192" s="10"/>
+      <c r="E192" s="10"/>
+      <c r="F192" s="10"/>
+      <c r="G192" s="10"/>
+      <c r="H192" s="10"/>
+      <c r="I192" s="10"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A193" s="36">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="B193" s="10"/>
+      <c r="C193" s="10"/>
+      <c r="D193" s="10"/>
+      <c r="E193" s="10"/>
+      <c r="F193" s="10"/>
+      <c r="G193" s="10"/>
+      <c r="H193" s="10"/>
+      <c r="I193" s="10"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A194" s="36">
+        <f t="shared" si="3"/>
+        <v>191</v>
+      </c>
+      <c r="B194" s="10"/>
+      <c r="C194" s="10"/>
+      <c r="D194" s="10"/>
+      <c r="E194" s="10"/>
+      <c r="F194" s="10"/>
+      <c r="G194" s="10"/>
+      <c r="H194" s="10"/>
+      <c r="I194" s="10"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A195" s="36">
+        <f t="shared" si="3"/>
+        <v>192</v>
+      </c>
+      <c r="B195" s="10"/>
+      <c r="C195" s="10"/>
+      <c r="D195" s="10"/>
+      <c r="E195" s="10"/>
+      <c r="F195" s="10"/>
+      <c r="G195" s="10"/>
+      <c r="H195" s="10"/>
+      <c r="I195" s="10"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A196" s="36">
+        <f t="shared" si="3"/>
+        <v>193</v>
+      </c>
+      <c r="B196" s="10"/>
+      <c r="C196" s="10"/>
+      <c r="D196" s="10"/>
+      <c r="E196" s="10"/>
+      <c r="F196" s="10"/>
+      <c r="G196" s="10"/>
+      <c r="H196" s="10"/>
+      <c r="I196" s="10"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A197" s="36">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="B197" s="10"/>
+      <c r="C197" s="10"/>
+      <c r="D197" s="10"/>
+      <c r="E197" s="10"/>
+      <c r="F197" s="10"/>
+      <c r="G197" s="10"/>
+      <c r="H197" s="10"/>
+      <c r="I197" s="10"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A198" s="36">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="B198" s="10"/>
+      <c r="C198" s="10"/>
+      <c r="D198" s="10"/>
+      <c r="E198" s="10"/>
+      <c r="F198" s="10"/>
+      <c r="G198" s="10"/>
+      <c r="H198" s="10"/>
+      <c r="I198" s="10"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A199" s="36">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="B199" s="10"/>
+      <c r="C199" s="10"/>
+      <c r="D199" s="10"/>
+      <c r="E199" s="10"/>
+      <c r="F199" s="10"/>
+      <c r="G199" s="10"/>
+      <c r="H199" s="10"/>
+      <c r="I199" s="10"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A200" s="36">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="B200" s="10"/>
+      <c r="C200" s="10"/>
+      <c r="D200" s="10"/>
+      <c r="E200" s="10"/>
+      <c r="F200" s="10"/>
+      <c r="G200" s="10"/>
+      <c r="H200" s="10"/>
+      <c r="I200" s="10"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A201" s="36">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="B201" s="10"/>
+      <c r="C201" s="10"/>
+      <c r="D201" s="10"/>
+      <c r="E201" s="10"/>
+      <c r="F201" s="10"/>
+      <c r="G201" s="10"/>
+      <c r="H201" s="10"/>
+      <c r="I201" s="10"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A202" s="36">
+        <f t="shared" si="3"/>
+        <v>199</v>
+      </c>
+      <c r="B202" s="10"/>
+      <c r="C202" s="10"/>
+      <c r="D202" s="10"/>
+      <c r="E202" s="10"/>
+      <c r="F202" s="10"/>
+      <c r="G202" s="10"/>
+      <c r="H202" s="10"/>
+      <c r="I202" s="10"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A203" s="36">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="B203" s="10"/>
+      <c r="C203" s="10"/>
+      <c r="D203" s="10"/>
+      <c r="E203" s="10"/>
+      <c r="F203" s="10"/>
+      <c r="G203" s="10"/>
+      <c r="H203" s="10"/>
+      <c r="I203" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>